<commit_message>
preenchimento do campo de prioridade
</commit_message>
<xml_diff>
--- a/Semestre 02/Analise e Projeto de Sistemas I/19.0220 Aula03/Sprint 2.xlsx
+++ b/Semestre 02/Analise e Projeto de Sistemas I/19.0220 Aula03/Sprint 2.xlsx
@@ -14,6 +14,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="165">
   <si>
+    <t>PERSONA</t>
+  </si>
+  <si>
+    <t>ID_HISTORIA_USUARIO</t>
+  </si>
+  <si>
+    <t>HISTORIA DE USUARIO</t>
+  </si>
+  <si>
+    <t>ID REGRA DE NEGOCIO</t>
+  </si>
+  <si>
     <t>Épico</t>
   </si>
   <si>
@@ -29,9 +41,6 @@
     <t>desejo</t>
   </si>
   <si>
-    <t>PERSONA</t>
-  </si>
-  <si>
     <t>para que eu possa</t>
   </si>
   <si>
@@ -50,111 +59,135 @@
     <t>acessar o aplicativo</t>
   </si>
   <si>
-    <t>ID_HISTORIA_USUARIO</t>
-  </si>
-  <si>
-    <t>HISTORIA DE USUARIO</t>
-  </si>
-  <si>
-    <t>ID REGRA DE NEGOCIO</t>
+    <t>ter acesso às suas funcionalidades</t>
+  </si>
+  <si>
+    <t>GHU1</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>realizar vendas</t>
+  </si>
+  <si>
+    <t>sustentar meu negócio</t>
+  </si>
+  <si>
+    <t>GHU2</t>
+  </si>
+  <si>
+    <t>disponibilizar descontos</t>
+  </si>
+  <si>
+    <t>alavancar vendas</t>
+  </si>
+  <si>
+    <t>GHU3</t>
+  </si>
+  <si>
+    <t>cadastrar e manipular produtos</t>
+  </si>
+  <si>
+    <t>controlar estoque e preços</t>
+  </si>
+  <si>
+    <t>GHU4</t>
+  </si>
+  <si>
+    <t>cadastrar e manipular metodos de pagamento</t>
+  </si>
+  <si>
+    <t>GHU5</t>
+  </si>
+  <si>
+    <t>emitir relatórios de vendas e estoque</t>
+  </si>
+  <si>
+    <t>realizar decisões informadas no negócio</t>
+  </si>
+  <si>
+    <t>GHU6</t>
+  </si>
+  <si>
+    <t>cadastrar valor de comissão em vendas</t>
+  </si>
+  <si>
+    <t>motivar meus funcionários</t>
+  </si>
+  <si>
+    <t>GHU7</t>
+  </si>
+  <si>
+    <t>ter uma conta admin no software</t>
+  </si>
+  <si>
+    <t>acessar funções especiais</t>
+  </si>
+  <si>
+    <t>VHU1</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>executar minha função</t>
+  </si>
+  <si>
+    <t>VHU2</t>
+  </si>
+  <si>
+    <t>cadastrar vendas</t>
+  </si>
+  <si>
+    <t>atualização de estoque e comissão</t>
+  </si>
+  <si>
+    <t>VHU3</t>
+  </si>
+  <si>
+    <t>consultar minha comissão</t>
+  </si>
+  <si>
+    <t>planejar meus gastos</t>
   </si>
   <si>
     <t>REGRA DE NEGOCIO</t>
   </si>
   <si>
-    <t>ter acesso às suas funcionalidades</t>
-  </si>
-  <si>
-    <t>GHU1</t>
-  </si>
-  <si>
-    <t>Gerente</t>
-  </si>
-  <si>
-    <t>realizar vendas</t>
-  </si>
-  <si>
-    <t>sustentar meu negócio</t>
-  </si>
-  <si>
-    <t>GHU2</t>
+    <t>VHU4</t>
   </si>
   <si>
     <t>GERENTE</t>
   </si>
   <si>
-    <t>disponibilizar descontos</t>
-  </si>
-  <si>
-    <t>alavancar vendas</t>
-  </si>
-  <si>
-    <t>GHU3</t>
-  </si>
-  <si>
-    <t>cadastrar e manipular produtos</t>
-  </si>
-  <si>
-    <t>controlar estoque e preços</t>
-  </si>
-  <si>
-    <t>GHU4</t>
-  </si>
-  <si>
-    <t>cadastrar e manipular metodos de pagamento</t>
-  </si>
-  <si>
-    <t>GHU5</t>
-  </si>
-  <si>
-    <t>emitir relatórios de vendas e estoque</t>
-  </si>
-  <si>
-    <t>realizar decisões informadas no negócio</t>
-  </si>
-  <si>
-    <t>GHU6</t>
-  </si>
-  <si>
-    <t>cadastrar valor de comissão em vendas</t>
-  </si>
-  <si>
-    <t>motivar meus funcionários</t>
+    <t>consultar estoque</t>
   </si>
   <si>
     <t>Eu como gerente quero realizar vendas para meus clientes</t>
   </si>
   <si>
-    <t>GHU7</t>
-  </si>
-  <si>
-    <t>ter uma conta admin no software</t>
-  </si>
-  <si>
-    <t>acessar funções especiais</t>
-  </si>
-  <si>
-    <t>VHU1</t>
-  </si>
-  <si>
     <t>RN1</t>
   </si>
   <si>
-    <t>Vendedor</t>
-  </si>
-  <si>
-    <t>executar minha função</t>
-  </si>
-  <si>
     <t>Ao Realizar uma venda e obrigatorio emissao de cupom fiscal</t>
   </si>
   <si>
-    <t>VHU2</t>
+    <t>VHU5</t>
+  </si>
+  <si>
+    <t>consultar vendas online</t>
+  </si>
+  <si>
+    <t>entregar produtos ao cliente</t>
   </si>
   <si>
     <t>RN2</t>
   </si>
   <si>
+    <t>VHU6</t>
+  </si>
+  <si>
     <t>A venda só e realizada após a confirmação do pagamento</t>
   </si>
   <si>
@@ -164,9 +197,6 @@
     <t>A venda só e realizada após a confirmação do estoque</t>
   </si>
   <si>
-    <t>cadastrar vendas</t>
-  </si>
-  <si>
     <t>RN4</t>
   </si>
   <si>
@@ -179,22 +209,22 @@
     <t>Ao ser efetuado uma compra com o metedo de pagamento no credito ou carne não podera ser parcelado acima de 5x</t>
   </si>
   <si>
-    <t>atualização de estoque e comissão</t>
-  </si>
-  <si>
     <t>RN6</t>
   </si>
   <si>
-    <t>VHU3</t>
+    <t>EHU1</t>
   </si>
   <si>
     <t>O Pagemento ao ser efetuado no boleto a vista tera 5% de desconto na compra</t>
   </si>
   <si>
-    <t>consultar minha comissão</t>
-  </si>
-  <si>
-    <t>planejar meus gastos</t>
+    <t>Estoquista</t>
+  </si>
+  <si>
+    <t>atualizar o estoque</t>
+  </si>
+  <si>
+    <t>manter a equipe informada</t>
   </si>
   <si>
     <t>RN7</t>
@@ -203,22 +233,61 @@
     <t>O Pagamento so podera ser parcelado caso seja Credito ou Carne</t>
   </si>
   <si>
-    <t>VHU4</t>
-  </si>
-  <si>
-    <t>consultar estoque</t>
-  </si>
-  <si>
-    <t>VHU5</t>
-  </si>
-  <si>
-    <t>consultar vendas online</t>
-  </si>
-  <si>
-    <t>entregar produtos ao cliente</t>
-  </si>
-  <si>
-    <t>VHU6</t>
+    <t>EHU2</t>
+  </si>
+  <si>
+    <t>ter acesso ao relatório de estoque</t>
+  </si>
+  <si>
+    <t>manter o gerente atualizado das necessidades</t>
+  </si>
+  <si>
+    <t>CHU1</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>realizar compras na loja fisica ou online</t>
+  </si>
+  <si>
+    <t>atender aos meus desejos</t>
+  </si>
+  <si>
+    <t>CHU2</t>
+  </si>
+  <si>
+    <t>consultar os metodos de pagamento</t>
+  </si>
+  <si>
+    <t>realizar compras com mais opções</t>
+  </si>
+  <si>
+    <t>CHU3</t>
+  </si>
+  <si>
+    <t>solicitar descontos em minhas compras</t>
+  </si>
+  <si>
+    <t>realizar compras mais eficientes</t>
+  </si>
+  <si>
+    <t>CHU4</t>
+  </si>
+  <si>
+    <t>me cadastrar</t>
+  </si>
+  <si>
+    <t>receber novas promoções</t>
+  </si>
+  <si>
+    <t>CHU5</t>
+  </si>
+  <si>
+    <t>retirar compras online na loja fisica</t>
+  </si>
+  <si>
+    <t>ter mais velocidade no processo de compra</t>
   </si>
   <si>
     <t>RN8</t>
@@ -227,85 +296,16 @@
     <t>A Venda so podera ser realizada com aprovação do cliente</t>
   </si>
   <si>
-    <t>EHU1</t>
-  </si>
-  <si>
-    <t>Estoquista</t>
-  </si>
-  <si>
-    <t>atualizar o estoque</t>
-  </si>
-  <si>
-    <t>manter a equipe informada</t>
-  </si>
-  <si>
-    <t>EHU2</t>
-  </si>
-  <si>
-    <t>ter acesso ao relatório de estoque</t>
-  </si>
-  <si>
     <t>RN9</t>
   </si>
   <si>
-    <t>manter o gerente atualizado das necessidades</t>
-  </si>
-  <si>
-    <t>CHU1</t>
-  </si>
-  <si>
     <t>A venda fisica so podera ser feita durante o horario de funcionamento da loja</t>
   </si>
   <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>realizar compras na loja fisica ou online</t>
-  </si>
-  <si>
-    <t>atender aos meus desejos</t>
-  </si>
-  <si>
-    <t>CHU2</t>
-  </si>
-  <si>
-    <t>consultar os metodos de pagamento</t>
-  </si>
-  <si>
-    <t>realizar compras com mais opções</t>
-  </si>
-  <si>
-    <t>CHU3</t>
-  </si>
-  <si>
-    <t>solicitar descontos em minhas compras</t>
-  </si>
-  <si>
-    <t>realizar compras mais eficientes</t>
-  </si>
-  <si>
-    <t>CHU4</t>
-  </si>
-  <si>
-    <t>me cadastrar</t>
-  </si>
-  <si>
     <t>RN10</t>
   </si>
   <si>
-    <t>receber novas promoções</t>
-  </si>
-  <si>
-    <t>CHU5</t>
-  </si>
-  <si>
     <t>Toda venda devera especificar sua Natureza (Online ou Fisica)</t>
-  </si>
-  <si>
-    <t>retirar compras online na loja fisica</t>
-  </si>
-  <si>
-    <t>ter mais velocidade no processo de compra</t>
   </si>
   <si>
     <t>Eu como gerente disponibilizarei descontos para meus clientes em algumas compras</t>
@@ -519,12 +519,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
     <font>
       <name val="Arial"/>
     </font>
@@ -572,16 +572,13 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -592,8 +589,8 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
@@ -601,16 +598,19 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -841,167 +841,167 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>44</v>
+      <c r="A2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3">
-      <c r="D3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>47</v>
+      <c r="D3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4">
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="D5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="D6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="D7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="D8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="7" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="A13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="7" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="14">
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="7" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="15">
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="7" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
         <v>108</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>109</v>
@@ -1031,19 +1031,19 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="A18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="7" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1095,7 +1095,7 @@
         <v>108</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>126</v>
@@ -1112,7 +1112,7 @@
         <v>108</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>129</v>
@@ -1146,7 +1146,7 @@
         <v>108</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>136</v>
@@ -1159,60 +1159,60 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="A26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="7" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27">
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="7" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="28">
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="7" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="29">
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="7" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="4" t="s">
+      <c r="A30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="7" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
         <v>108</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>150</v>
@@ -1234,19 +1234,19 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="A32" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="7" t="s">
         <v>155</v>
       </c>
     </row>
@@ -1320,323 +1320,386 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="H6" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="F10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="C9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="H13" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="C10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="C11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="E14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="C12" s="1" t="s">
+      <c r="H14" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="C13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="D15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="C15" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="E16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="C17" s="1" t="s">
+      <c r="F17" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="H17" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="C18" s="1" t="s">
+      <c r="F18" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="H18" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="H19" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="C19" s="1" t="s">
+      <c r="D20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="H20" s="2">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="C20" s="1" t="s">
+      <c r="D21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="H21" s="2">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="C21" s="1" t="s">
+      <c r="D22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>97</v>
+      <c r="H22" s="2">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>